<commit_message>
Updated excel file and readme
</commit_message>
<xml_diff>
--- a/assignment.xlsx
+++ b/assignment.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalgajurel/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalgajurel/Documents/Works/InsuranceQuestionnaireAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D46EBC-AD2C-314F-AD67-ABCA375C4B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59714F87-669D-F74C-BA6C-DABB4329EBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" activeTab="1" xr2:uid="{FEA8CFEE-0782-7F46-B574-5029635569FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Collected Questions" sheetId="3" r:id="rId1"/>
-    <sheet name="Carrier Comparision" sheetId="1" r:id="rId2"/>
+    <sheet name="Question Analysis" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>SN</t>
   </si>
@@ -228,12 +228,6 @@
     <t>Similar Questions (A And B)</t>
   </si>
   <si>
-    <t>A - B</t>
-  </si>
-  <si>
-    <t>Questions uniqe to Carrier A</t>
-  </si>
-  <si>
     <t>1. What is the zip code of your primary business location?
 2. What kind of work do you do?
 3. What is the name of your business? (conditioned: if DBA then take DBA also.)
@@ -258,12 +252,15 @@
 24. Do you hire other labor beside your employee?(Pick Yes/No)
 25. How many branches do you have? (Number)</t>
   </si>
+  <si>
+    <t>Choice Type Table</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -318,6 +315,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -351,23 +355,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -379,11 +374,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,327 +715,328 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE4061-8584-6049-AD29-B56C5FE3B83B}">
   <dimension ref="C3:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScale="50" zoomScaleNormal="37" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C31"/>
+    <sheetView zoomScale="41" zoomScaleNormal="37" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="255.6640625" customWidth="1"/>
     <col min="4" max="4" width="203.5" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="C3" s="12" t="s">
+    <row r="3" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="3:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="3:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="3:12" ht="31" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="3:12" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+      <c r="E6" s="8"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="3:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="2"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="2"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="2"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="2"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="2"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="2"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="2"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="2"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="2"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="2"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="2"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="2"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="2"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="2"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="2"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="2"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="2"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="2"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="2"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="2"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="2"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="2"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="2"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="2"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
+      <c r="D7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="15"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="15"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="15"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="15"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="15"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="15"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="15"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="15"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="15"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="15"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="15"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="15"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="15"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="15"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="15"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="15"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="15"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="15"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="15"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="15"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="15"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="15"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="15"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="15"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C3:K5"/>
     <mergeCell ref="C7:C31"/>
     <mergeCell ref="D7:D31"/>
+    <mergeCell ref="C3:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1029,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6D63A8-C638-2F41-93A8-DECB302FE352}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D5" sqref="D5:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1040,64 +1055,66 @@
     <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="88.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="8"/>
-    <col min="7" max="7" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="18.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
+    <row r="2" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1"/>
       <c r="D2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="14"/>
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="17"/>
+      <c r="F3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="7"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1107,7 +1124,7 @@
       <c r="D4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1131,16 +1148,16 @@
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1154,22 +1171,22 @@
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1183,19 +1200,19 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="2">
         <v>3</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1209,22 +1226,22 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="2">
         <v>4</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1238,16 +1255,16 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1261,16 +1278,16 @@
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="2">
         <v>6</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1284,19 +1301,19 @@
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="2">
         <v>7</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1310,16 +1327,16 @@
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="2">
         <v>8</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1333,16 +1350,16 @@
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="2">
         <v>9</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1356,19 +1373,19 @@
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1382,16 +1399,16 @@
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="2">
         <v>11</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1405,16 +1422,16 @@
       <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="2">
         <v>12</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1428,48 +1445,39 @@
       <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="2">
         <v>13</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="F3:F4"/>
+  <mergeCells count="9">
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final changes and commit
</commit_message>
<xml_diff>
--- a/assignment.xlsx
+++ b/assignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalgajurel/Documents/Works/InsuranceQuestionnaireAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59714F87-669D-F74C-BA6C-DABB4329EBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE478AB4-FCBC-F242-8585-3C685B853C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" activeTab="1" xr2:uid="{FEA8CFEE-0782-7F46-B574-5029635569FC}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" xr2:uid="{FEA8CFEE-0782-7F46-B574-5029635569FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Collected Questions" sheetId="3" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>Do you hire other labor beside your employee?</t>
   </si>
   <si>
-    <t>How many branches do you have?</t>
-  </si>
-  <si>
     <t>Employee Compensation  Questions</t>
   </si>
   <si>
@@ -228,6 +225,12 @@
     <t>Similar Questions (A And B)</t>
   </si>
   <si>
+    <t>Choice Type Table</t>
+  </si>
+  <si>
+    <t>Do you have 2 or more branches?</t>
+  </si>
+  <si>
     <t>1. What is the zip code of your primary business location?
 2. What kind of work do you do?
 3. What is the name of your business? (conditioned: if DBA then take DBA also.)
@@ -250,10 +253,7 @@
 22. Is workers' compensation coverage currently in effect? (Pick Yes/No)
 23. Has your workers' compensation coverage been declined, canceled, or non-renewed within the last 3 years? (Pick Yes/No)
 24. Do you hire other labor beside your employee?(Pick Yes/No)
-25. How many branches do you have? (Number)</t>
-  </si>
-  <si>
-    <t>Choice Type Table</t>
+25. Do you have 2 or more branches??(Pick Yes/No)</t>
   </si>
 </sst>
 </file>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE4061-8584-6049-AD29-B56C5FE3B83B}">
   <dimension ref="C3:L31"/>
   <sheetViews>
-    <sheetView zoomScale="41" zoomScaleNormal="37" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D6"/>
+    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="37" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,7 +728,7 @@
   <sheetData>
     <row r="3" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="16"/>
@@ -766,10 +766,10 @@
     </row>
     <row r="6" spans="3:12" ht="31" x14ac:dyDescent="0.25">
       <c r="C6" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="8"/>
       <c r="H6" s="5"/>
@@ -780,10 +780,10 @@
     </row>
     <row r="7" spans="3:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E7" s="15"/>
       <c r="H7" s="5"/>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6D63A8-C638-2F41-93A8-DECB302FE352}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D17"/>
+    <sheetView zoomScale="72" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1065,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="7"/>
@@ -1083,7 +1083,7 @@
       <c r="C2" s="1"/>
       <c r="D2"/>
       <c r="F2" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="14" t="s">
@@ -1122,7 +1122,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3" t="s">
@@ -1149,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -1172,7 +1172,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
@@ -1201,7 +1201,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="2">
         <v>3</v>
@@ -1227,7 +1227,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="2">
         <v>4</v>
@@ -1256,7 +1256,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
@@ -1279,7 +1279,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="2">
         <v>6</v>
@@ -1302,7 +1302,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2">
         <v>7</v>
@@ -1328,7 +1328,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2">
         <v>8</v>
@@ -1351,7 +1351,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2">
         <v>9</v>
@@ -1374,7 +1374,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
@@ -1400,7 +1400,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2">
         <v>11</v>
@@ -1423,7 +1423,7 @@
         <v>43</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2">
         <v>12</v>
@@ -1443,10 +1443,10 @@
         <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2">
         <v>13</v>

</xml_diff>

<commit_message>
Fixed typo and other mistakes
</commit_message>
<xml_diff>
--- a/assignment.xlsx
+++ b/assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kushalgajurel/Documents/Works/InsuranceQuestionnaireAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE478AB4-FCBC-F242-8585-3C685B853C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6056F5-DE43-D04A-B3BD-1C1B8997C6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" xr2:uid="{FEA8CFEE-0782-7F46-B574-5029635569FC}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t>What date did your business begin under current ownership?</t>
   </si>
   <si>
-    <t>In the past 3 years how many Workers' Compensation claims were reported?</t>
-  </si>
-  <si>
     <t>Has your company had any claims in the past 5 years?</t>
   </si>
   <si>
@@ -191,32 +188,6 @@
   </si>
   <si>
     <t>Carrier A</t>
-  </si>
-  <si>
-    <t>1. Zip Code?
-2. What's your industry?
-3. Do you have any employees?
-4. How many employees do you have? (Include both part-time and full-time employees in your response. Exclude business owners and officers.)
-5. Where does your business operate? (If you lease space on an ongoing basis but also work from home or a job site, select "I lease space from others." If you work from home but also have a temporary space lease or work from a job site, select "I run my business out of my home.")
-6. Where is your business located?
-7. When did you start your business? (Drop Down - Brand New, Started last year, Started 2 years......., started 10 or more years)
-8. How is your business structured? (Drop Down - Corporation, Partnership, Individual/Sole Proprietor, Sub-Chapter Corp)
-9. Do you want to include coverage for any owners/officers? (Drop Down - No, Yes buy coverage for 1 owner/officer........., Yes buy coverage for 5 or more owners/officers)
-10. Do any staff install computer hardware at client locations? (Yes/No)
-11. Do any employees travel frequently for sales, consultation, or programming? (Yes/No)
-12. Do you provide any staffing services? (Yes/No)
-13. In the past 3 years how many Workers' Compensation claims were reported? (Drop Down - None, 1 .... 6 or more)
-14. Do you use any volunteers or donated labor? (Yes/No)
-15. Do you have multiple locations in more than one state? (Yes/No)
-16. Insured first name
-17. Insured last name
-18. Doing business as (optional)
-19. Business website (optional)
-20. Business address line 1
-21. Business address line 2
-22. City (Drop Down based in Zip Code)
-23. Contact email
-24. Contact phone</t>
   </si>
   <si>
     <t>Carrier B</t>
@@ -254,6 +225,35 @@
 23. Has your workers' compensation coverage been declined, canceled, or non-renewed within the last 3 years? (Pick Yes/No)
 24. Do you hire other labor beside your employee?(Pick Yes/No)
 25. Do you have 2 or more branches??(Pick Yes/No)</t>
+  </si>
+  <si>
+    <t>In the past 3 years were any Workers' Compensation claims reported?</t>
+  </si>
+  <si>
+    <t>1. Zip Code?
+2. What's your industry?
+3. Do you have any employees?
+4. How many employees do you have? (Include both part-time and full-time employees in your response. Exclude business owners and officers.)
+5. Where does your business operate? (If you lease space on an ongoing basis but also work from home or a job site, select "I lease space from others." If you work from home but also have a temporary space lease or work from a job site, select "I run my business out of my home.")
+6. Where is your business located?
+7. When did you start your business? (Drop Down - Brand New, Started last year, Started 2 years......., started 10 or more years)
+8. How is your business structured? (Drop Down - Corporation, Partnership, Individual/Sole Proprietor, Sub-Chapter Corp)
+9. Do you want to include coverage for any owners/officers? (Drop Down - No, Yes buy coverage for 1 owner/officer........., Yes buy coverage for 5 or more owners/officers)
+10. Do any staff install computer hardware at client locations? (Yes/No)
+11. Do any employees travel frequently for sales, consultation, or programming? (Yes/No)
+12. Do you provide any staffing services? (Yes/No)
+13. In the past 3 years were any Workers' Compensation claims reported?
+14. Do you use any volunteers or donated labor? (Yes/No)
+15. Do you have multiple locations in more than one state? (Yes/No)
+16. Insured first name
+17. Insured last name
+18. Doing business as (optional)
+19. Business website (optional)
+20. Business address line 1
+21. Business address line 2
+22. City (Drop Down based in Zip Code)
+23. Contact email
+24. Contact phone</t>
   </si>
 </sst>
 </file>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE4061-8584-6049-AD29-B56C5FE3B83B}">
   <dimension ref="C3:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="37" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="41" zoomScaleNormal="37" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,7 +728,7 @@
   <sheetData>
     <row r="3" spans="3:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="16"/>
@@ -766,10 +766,10 @@
     </row>
     <row r="6" spans="3:12" ht="31" x14ac:dyDescent="0.25">
       <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="E6" s="8"/>
       <c r="H6" s="5"/>
@@ -780,10 +780,10 @@
     </row>
     <row r="7" spans="3:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="15"/>
       <c r="H7" s="5"/>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1065,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="7"/>
@@ -1083,7 +1083,7 @@
       <c r="C2" s="1"/>
       <c r="D2"/>
       <c r="F2" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="14" t="s">
@@ -1122,20 +1122,20 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1149,16 +1149,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1166,28 +1166,28 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1201,19 +1201,19 @@
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2">
         <v>3</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1227,22 +1227,22 @@
         <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2">
         <v>4</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1256,16 +1256,16 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1279,16 +1279,16 @@
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="2">
         <v>6</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1299,22 +1299,22 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="2">
         <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1328,16 +1328,16 @@
         <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="2">
         <v>8</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1351,16 +1351,16 @@
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="2">
         <v>9</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1374,19 +1374,19 @@
         <v>20</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1394,22 +1394,22 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2">
         <v>11</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1417,22 +1417,22 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="2">
         <v>12</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1440,22 +1440,22 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2">
         <v>13</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>